<commit_message>
pre-2018 decisions, as well as post-2018 updated demands, optimal prices, but no decisions yet. also updated readme to be comprehensive
</commit_message>
<xml_diff>
--- a/decisions/notgrapefruit2019_4test_tweak.xlsx
+++ b/decisions/notgrapefruit2019_4test_tweak.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="basic_info" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="shipping_manufacturing" sheetId="4" r:id="rId4"/>
     <sheet name="pricing" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -635,7 +632,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -912,28 +909,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -959,7 +934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1049,7 +1024,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
@@ -1058,9 +1032,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1116,33 +1088,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="basic_info"/>
-      <sheetName val="facilities"/>
-      <sheetName val="raw_materials"/>
-      <sheetName val="shipping_manufacturing"/>
-      <sheetName val="pricing"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="D5">
-            <v>2018</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1433,22 +1378,22 @@
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="98"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="95"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="99">
+      <c r="D5" s="96">
         <v>2019</v>
       </c>
-      <c r="E5" s="100"/>
-      <c r="F5" s="101"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -1470,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2470,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="D51" s="14">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>11</v>
@@ -2480,7 +2425,7 @@
       </c>
       <c r="G51" s="16">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H51" s="18" t="str">
         <f t="shared" si="4"/>
@@ -2874,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="16">
-        <v>3300</v>
+        <v>4000</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>11</v>
@@ -2884,7 +2829,7 @@
       </c>
       <c r="G66" s="16">
         <f t="shared" si="3"/>
-        <v>3300</v>
+        <v>4000</v>
       </c>
       <c r="H66" s="18" t="str">
         <f t="shared" si="4"/>
@@ -3089,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="D74" s="16">
-        <v>850</v>
+        <v>1250</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>11</v>
@@ -3099,7 +3044,7 @@
       </c>
       <c r="G74" s="16">
         <f t="shared" si="3"/>
-        <v>850</v>
+        <v>1250</v>
       </c>
       <c r="H74" s="18" t="str">
         <f t="shared" si="4"/>
@@ -3439,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="D87" s="16">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="E87" s="16" t="s">
         <v>11</v>
@@ -3449,7 +3394,7 @@
       </c>
       <c r="G87" s="16">
         <f t="shared" si="3"/>
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="H87" s="18" t="str">
         <f t="shared" si="4"/>
@@ -4009,8 +3954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4734,33 +4679,33 @@
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
       <c r="D28" s="55">
-        <f>[1]basic_info!$D$5-5</f>
-        <v>2013</v>
+        <f>basic_info!$D$5-5</f>
+        <v>2014</v>
       </c>
       <c r="E28" s="52"/>
       <c r="F28" s="55">
-        <f>[1]basic_info!$D$5-4</f>
-        <v>2014</v>
+        <f>basic_info!$D$5-4</f>
+        <v>2015</v>
       </c>
       <c r="G28" s="52"/>
       <c r="H28" s="55">
-        <f>[1]basic_info!$D$5-3</f>
-        <v>2015</v>
+        <f>basic_info!$D$5-3</f>
+        <v>2016</v>
       </c>
       <c r="I28" s="52"/>
       <c r="J28" s="55">
-        <f>[1]basic_info!$D$5-2</f>
-        <v>2016</v>
+        <f>basic_info!$D$5-2</f>
+        <v>2017</v>
       </c>
       <c r="K28" s="52"/>
       <c r="L28" s="55">
-        <f>[1]basic_info!$D$5-1</f>
-        <v>2017</v>
+        <f>basic_info!$D$5-1</f>
+        <v>2018</v>
       </c>
       <c r="M28" s="32"/>
       <c r="N28" s="55">
-        <f>[1]basic_info!$D$5</f>
-        <v>2018</v>
+        <f>basic_info!$D$5</f>
+        <v>2019</v>
       </c>
       <c r="O28" s="32"/>
       <c r="P28" s="51"/>
@@ -4818,9 +4763,9 @@
       <c r="B30" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="40">
-        <f>[1]basic_info!$D$5</f>
-        <v>2018</v>
+      <c r="C30" s="55">
+        <f>basic_info!$D$5</f>
+        <v>2019</v>
       </c>
       <c r="D30" s="56">
         <v>0.68616087553988669</v>
@@ -4860,9 +4805,9 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="32"/>
       <c r="B31" s="40"/>
-      <c r="C31" s="57">
-        <f>[1]basic_info!$D$5+1</f>
-        <v>2019</v>
+      <c r="C31" s="55">
+        <f>basic_info!$D$5+1</f>
+        <v>2020</v>
       </c>
       <c r="D31" s="61"/>
       <c r="E31" s="62"/>
@@ -4898,9 +4843,9 @@
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="32"/>
       <c r="B32" s="40"/>
-      <c r="C32" s="57">
-        <f>[1]basic_info!$D$5+2</f>
-        <v>2020</v>
+      <c r="C32" s="55">
+        <f>basic_info!$D$5+2</f>
+        <v>2021</v>
       </c>
       <c r="D32" s="61"/>
       <c r="E32" s="62"/>
@@ -4932,9 +4877,9 @@
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="32"/>
       <c r="B33" s="40"/>
-      <c r="C33" s="57">
-        <f>[1]basic_info!$D$5+3</f>
-        <v>2021</v>
+      <c r="C33" s="55">
+        <f>basic_info!$D$5+3</f>
+        <v>2022</v>
       </c>
       <c r="D33" s="61"/>
       <c r="E33" s="62"/>
@@ -4962,9 +4907,9 @@
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="32"/>
       <c r="B34" s="40"/>
-      <c r="C34" s="57">
-        <f>[1]basic_info!$D$5+4</f>
-        <v>2022</v>
+      <c r="C34" s="55">
+        <f>basic_info!$D$5+4</f>
+        <v>2023</v>
       </c>
       <c r="D34" s="61"/>
       <c r="E34" s="62"/>
@@ -4990,25 +4935,25 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="32"/>
       <c r="B35" s="43"/>
-      <c r="C35" s="69">
-        <f>[1]basic_info!$D$5+5</f>
-        <v>2023</v>
-      </c>
-      <c r="D35" s="70"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="72"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="74">
+      <c r="C35" s="55">
+        <f>basic_info!$D$5+5</f>
+        <v>2024</v>
+      </c>
+      <c r="D35" s="69"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="73">
         <v>0.68592924540042888</v>
       </c>
       <c r="O35" s="68"/>
-      <c r="P35" s="75">
+      <c r="P35" s="74">
         <f>O35</f>
         <v>0</v>
       </c>
@@ -5018,37 +4963,35 @@
       <c r="B36" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="40">
-        <f>[1]basic_info!$D$5</f>
-        <v>2018</v>
-      </c>
-      <c r="D36" s="56">
-        <v>1.0288140534879155</v>
+      <c r="C36" s="55">
+        <f>basic_info!$D$5</f>
+        <v>2019</v>
+      </c>
+      <c r="D36" s="63">
+        <v>0.98955166281759732</v>
       </c>
       <c r="E36" s="39">
         <v>0</v>
       </c>
-      <c r="F36" s="76">
-        <v>1.0108999284690923</v>
-      </c>
-      <c r="G36" s="77">
-        <v>0</v>
-      </c>
-      <c r="H36" s="76">
-        <v>1.0032828986441651</v>
-      </c>
-      <c r="I36" s="77">
+      <c r="F36" s="65">
+        <v>0.95103433990902408</v>
+      </c>
+      <c r="G36" s="66">
         <v>136000</v>
       </c>
-      <c r="J36" s="76">
-        <v>1.0357981248188022</v>
-      </c>
-      <c r="K36" s="77"/>
-      <c r="L36" s="78">
+      <c r="H36" s="65">
+        <v>0.9919351074281193</v>
+      </c>
+      <c r="I36" s="66"/>
+      <c r="J36" s="65">
+        <v>0.94692158975803442</v>
+      </c>
+      <c r="K36" s="66"/>
+      <c r="L36" s="75">
         <v>0.97406708065219405</v>
       </c>
-      <c r="M36" s="79"/>
-      <c r="N36" s="80"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="77"/>
       <c r="O36" s="60" t="s">
         <v>134</v>
       </c>
@@ -5060,34 +5003,32 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="32"/>
       <c r="B37" s="40"/>
-      <c r="C37" s="57">
-        <f>[1]basic_info!$D$5+1</f>
-        <v>2019</v>
+      <c r="C37" s="55">
+        <f>basic_info!$D$5+1</f>
+        <v>2020</v>
       </c>
       <c r="D37" s="61"/>
       <c r="E37" s="62"/>
       <c r="F37" s="63">
-        <v>0.98955166281759732</v>
+        <v>0.9180320969671012</v>
       </c>
       <c r="G37" s="64">
-        <v>0</v>
+        <v>136000</v>
       </c>
       <c r="H37" s="65">
-        <v>0.95103433990902408</v>
-      </c>
-      <c r="I37" s="66">
-        <v>136000</v>
-      </c>
+        <v>0.95493263137485418</v>
+      </c>
+      <c r="I37" s="66"/>
       <c r="J37" s="65">
-        <v>0.9919351074281193</v>
+        <v>0.93709078332824058</v>
       </c>
       <c r="K37" s="66"/>
       <c r="L37" s="65">
-        <v>0.94692158975803442</v>
+        <v>1.2538421609133918</v>
       </c>
       <c r="M37" s="66"/>
       <c r="N37" s="65">
-        <v>1.3519645777200024</v>
+        <v>0.97406708065219405</v>
       </c>
       <c r="O37" s="68"/>
       <c r="P37" s="67">
@@ -5098,43 +5039,43 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
       <c r="B38" s="40"/>
-      <c r="C38" s="57">
-        <f>[1]basic_info!$D$5+2</f>
-        <v>2020</v>
+      <c r="C38" s="55">
+        <f>basic_info!$D$5+2</f>
+        <v>2021</v>
       </c>
       <c r="D38" s="61"/>
       <c r="E38" s="62"/>
       <c r="F38" s="62"/>
       <c r="G38" s="62"/>
       <c r="H38" s="63">
-        <v>0.9180320969671012</v>
+        <v>0.9100411573201419</v>
       </c>
       <c r="I38" s="64">
-        <v>136000</v>
+        <v>89461</v>
       </c>
       <c r="J38" s="65">
-        <v>0.95493263137485418</v>
+        <v>0.92721692835977987</v>
       </c>
       <c r="K38" s="66"/>
       <c r="L38" s="65">
-        <v>0.93709078332824058</v>
+        <v>1.1631721092862846</v>
       </c>
       <c r="M38" s="66"/>
       <c r="N38" s="65">
-        <v>1.2538421609133918</v>
+        <v>0.94692158975803442</v>
       </c>
       <c r="O38" s="68"/>
       <c r="P38" s="67">
         <f>O38+M38+K38+I38</f>
-        <v>136000</v>
+        <v>89461</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="32"/>
       <c r="B39" s="40"/>
-      <c r="C39" s="57">
-        <f>[1]basic_info!$D$5+3</f>
-        <v>2021</v>
+      <c r="C39" s="55">
+        <f>basic_info!$D$5+3</f>
+        <v>2022</v>
       </c>
       <c r="D39" s="61"/>
       <c r="E39" s="62"/>
@@ -5143,17 +5084,17 @@
       <c r="H39" s="62"/>
       <c r="I39" s="62"/>
       <c r="J39" s="63">
-        <v>0.9100411573201419</v>
+        <v>0.89172850017249583</v>
       </c>
       <c r="K39" s="64">
         <v>89461</v>
       </c>
       <c r="L39" s="65">
-        <v>0.92721692835977987</v>
+        <v>1.1067776852666162</v>
       </c>
       <c r="M39" s="66"/>
       <c r="N39" s="65">
-        <v>1.1631721092862846</v>
+        <v>0.93709078332824058</v>
       </c>
       <c r="O39" s="68"/>
       <c r="P39" s="67">
@@ -5164,9 +5105,9 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="32"/>
       <c r="B40" s="40"/>
-      <c r="C40" s="57">
-        <f>[1]basic_info!$D$5+4</f>
-        <v>2022</v>
+      <c r="C40" s="55">
+        <f>basic_info!$D$5+4</f>
+        <v>2023</v>
       </c>
       <c r="D40" s="61"/>
       <c r="E40" s="62"/>
@@ -5177,44 +5118,44 @@
       <c r="J40" s="62"/>
       <c r="K40" s="62"/>
       <c r="L40" s="63">
-        <v>0.89172850017249583</v>
+        <v>1.0097698285728693</v>
       </c>
       <c r="M40" s="64">
-        <v>89461</v>
+        <v>107018.3</v>
       </c>
       <c r="N40" s="65">
-        <v>1.1067776852666162</v>
+        <v>0.92721692835977987</v>
       </c>
       <c r="O40" s="68"/>
       <c r="P40" s="67">
         <f>O40+M40</f>
-        <v>89461</v>
+        <v>107018.3</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="32"/>
       <c r="B41" s="43"/>
-      <c r="C41" s="69">
-        <f>[1]basic_info!$D$5+5</f>
-        <v>2023</v>
-      </c>
-      <c r="D41" s="70"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="72"/>
-      <c r="M41" s="73"/>
+      <c r="C41" s="55">
+        <f>basic_info!$D$5+5</f>
+        <v>2024</v>
+      </c>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="72"/>
       <c r="N41" s="63">
-        <v>1.0097698285728693</v>
+        <v>0.89172850017249583</v>
       </c>
       <c r="O41" s="68">
         <v>107018.3</v>
       </c>
-      <c r="P41" s="74">
+      <c r="P41" s="73">
         <f>O41</f>
         <v>107018.3</v>
       </c>
@@ -5344,51 +5285,51 @@
       <c r="B47" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="81">
+      <c r="C47" s="78">
         <f t="shared" ref="C47:N48" si="0">100/12</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="D47" s="81">
+      <c r="D47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="E47" s="81">
+      <c r="E47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="F47" s="81">
+      <c r="F47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G47" s="81">
+      <c r="G47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="H47" s="81">
+      <c r="H47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="I47" s="81">
+      <c r="I47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="J47" s="81">
+      <c r="J47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="K47" s="81">
+      <c r="K47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="L47" s="81">
+      <c r="L47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="M47" s="81">
+      <c r="M47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="N47" s="81">
+      <c r="N47" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
@@ -5403,51 +5344,51 @@
       <c r="B48" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="81">
+      <c r="C48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="D48" s="81">
+      <c r="D48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="E48" s="81">
+      <c r="E48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="F48" s="81">
+      <c r="F48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G48" s="81">
+      <c r="G48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="H48" s="81">
+      <c r="H48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="I48" s="81">
+      <c r="I48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="J48" s="81">
+      <c r="J48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="K48" s="81">
+      <c r="K48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="L48" s="81">
+      <c r="L48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="M48" s="81">
+      <c r="M48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="N48" s="81">
+      <c r="N48" s="78">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
@@ -5511,7 +5452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -5571,16 +5512,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="32"/>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
       <c r="L4" s="52"/>
       <c r="M4" s="52"/>
       <c r="N4" s="52"/>
@@ -5626,27 +5567,27 @@
       <c r="B6" s="55" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83">
+      <c r="C6" s="80"/>
+      <c r="D6" s="80">
         <f>0.273797 * 100</f>
         <v>27.3797</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83">
+      <c r="E6" s="80"/>
+      <c r="F6" s="80">
         <f>0.08137569 * 100</f>
         <v>8.1375689999999992</v>
       </c>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83">
+      <c r="G6" s="80"/>
+      <c r="H6" s="80">
         <f xml:space="preserve"> 0.4674289*100</f>
         <v>46.742889999999996</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83">
+      <c r="I6" s="80"/>
+      <c r="J6" s="80">
         <f>100-SUM(C6:I6)</f>
         <v>17.739841000000013</v>
       </c>
-      <c r="K6" s="84">
+      <c r="K6" s="81">
         <f>SUM($C$6:$J$6)</f>
         <v>100</v>
       </c>
@@ -5659,23 +5600,23 @@
       <c r="B7" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83">
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80">
         <f>0.42008*100</f>
         <v>42.008000000000003</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83">
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80">
         <f>0.57992*100</f>
         <v>57.991999999999997</v>
       </c>
-      <c r="J7" s="83">
-        <v>0</v>
-      </c>
-      <c r="K7" s="84">
+      <c r="J7" s="80">
+        <v>0</v>
+      </c>
+      <c r="K7" s="81">
         <f>SUM($C$7:$J$7)</f>
         <v>100</v>
       </c>
@@ -5688,23 +5629,23 @@
       <c r="B8" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="80">
         <f>0.4678839*100</f>
         <v>46.78839</v>
       </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83">
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80">
         <f>0.5321161*100</f>
         <v>53.21161</v>
       </c>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83">
-        <v>0</v>
-      </c>
-      <c r="K8" s="84">
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80">
+        <v>0</v>
+      </c>
+      <c r="K8" s="81">
         <f>SUM($C$8:$J$8)</f>
         <v>100</v>
       </c>
@@ -5717,19 +5658,19 @@
       <c r="B9" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="83">
+      <c r="C9" s="80">
         <v>100</v>
       </c>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83">
-        <v>0</v>
-      </c>
-      <c r="K9" s="84">
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80">
+        <v>0</v>
+      </c>
+      <c r="K9" s="81">
         <f>SUM($C$9:$J$9)</f>
         <v>100</v>
       </c>
@@ -5742,19 +5683,19 @@
       <c r="B10" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="83">
+      <c r="C10" s="80">
         <v>100</v>
       </c>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83">
-        <v>0</v>
-      </c>
-      <c r="K10" s="84">
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80">
+        <v>0</v>
+      </c>
+      <c r="K10" s="81">
         <f>SUM($C$10:$J$10)</f>
         <v>100</v>
       </c>
@@ -5767,19 +5708,19 @@
       <c r="B11" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="82">
         <v>100</v>
       </c>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="83">
-        <v>0</v>
-      </c>
-      <c r="K11" s="86">
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="80">
+        <v>0</v>
+      </c>
+      <c r="K11" s="83">
         <f>SUM($C$11:$J$11)</f>
         <v>100</v>
       </c>
@@ -5821,7 +5762,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="84" t="s">
         <v>142</v>
       </c>
       <c r="C14" s="52"/>
@@ -5839,7 +5780,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="85" t="s">
         <v>143</v>
       </c>
       <c r="C15" s="51"/>
@@ -5936,7 +5877,7 @@
       <c r="B19" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="C19" s="85">
+      <c r="C19" s="82">
         <f>0.7273768*100</f>
         <v>72.737680000000012</v>
       </c>
@@ -5944,7 +5885,7 @@
         <f>100-$C$19</f>
         <v>27.262319999999988</v>
       </c>
-      <c r="E19" s="85">
+      <c r="E19" s="82">
         <f>0.5806958*100</f>
         <v>58.069580000000002</v>
       </c>
@@ -5952,7 +5893,7 @@
         <f>100-$E$19</f>
         <v>41.930419999999998</v>
       </c>
-      <c r="G19" s="85">
+      <c r="G19" s="82">
         <f>0.5135476*100</f>
         <v>51.354759999999999</v>
       </c>
@@ -5960,7 +5901,7 @@
         <f>100-$G$19</f>
         <v>48.645240000000001</v>
       </c>
-      <c r="I19" s="85">
+      <c r="I19" s="82">
         <f>0.5466106*100</f>
         <v>54.661059999999992</v>
       </c>
@@ -5975,15 +5916,15 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="89"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
       <c r="K20" s="51"/>
       <c r="L20" s="51"/>
       <c r="M20" s="51"/>
@@ -6007,7 +5948,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="32"/>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="84" t="s">
         <v>138</v>
       </c>
       <c r="C22" s="32"/>
@@ -6025,7 +5966,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="32"/>
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="87" t="s">
         <v>149</v>
       </c>
       <c r="C23" s="32"/>
@@ -6126,32 +6067,32 @@
       <c r="B27" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="83">
+      <c r="C27" s="80">
         <f>0.1860653*100</f>
         <v>18.606529999999999</v>
       </c>
-      <c r="D27" s="83">
+      <c r="D27" s="80">
         <v>100</v>
       </c>
-      <c r="E27" s="83">
+      <c r="E27" s="80">
         <v>100</v>
       </c>
-      <c r="F27" s="83">
-        <v>0</v>
-      </c>
-      <c r="G27" s="83">
-        <v>0</v>
-      </c>
-      <c r="H27" s="83">
-        <v>0</v>
-      </c>
-      <c r="I27" s="83">
-        <v>0</v>
-      </c>
-      <c r="J27" s="83">
-        <v>0</v>
-      </c>
-      <c r="K27" s="91">
+      <c r="F27" s="80">
+        <v>0</v>
+      </c>
+      <c r="G27" s="80">
+        <v>0</v>
+      </c>
+      <c r="H27" s="80">
+        <v>0</v>
+      </c>
+      <c r="I27" s="80">
+        <v>0</v>
+      </c>
+      <c r="J27" s="80">
+        <v>0</v>
+      </c>
+      <c r="K27" s="88">
         <v>0</v>
       </c>
       <c r="L27" s="32"/>
@@ -6163,32 +6104,32 @@
       <c r="B28" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="83">
+      <c r="C28" s="80">
         <f>0.4702319*100</f>
         <v>47.02319</v>
       </c>
-      <c r="D28" s="83">
-        <v>0</v>
-      </c>
-      <c r="E28" s="83">
-        <v>0</v>
-      </c>
-      <c r="F28" s="83">
+      <c r="D28" s="80">
+        <v>0</v>
+      </c>
+      <c r="E28" s="80">
+        <v>0</v>
+      </c>
+      <c r="F28" s="80">
         <v>100</v>
       </c>
-      <c r="G28" s="83">
+      <c r="G28" s="80">
         <v>100</v>
       </c>
-      <c r="H28" s="83">
-        <v>0</v>
-      </c>
-      <c r="I28" s="83">
-        <v>0</v>
-      </c>
-      <c r="J28" s="83">
-        <v>0</v>
-      </c>
-      <c r="K28" s="91">
+      <c r="H28" s="80">
+        <v>0</v>
+      </c>
+      <c r="I28" s="80">
+        <v>0</v>
+      </c>
+      <c r="J28" s="80">
+        <v>0</v>
+      </c>
+      <c r="K28" s="88">
         <v>0</v>
       </c>
       <c r="L28" s="32"/>
@@ -6200,32 +6141,32 @@
       <c r="B29" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="83">
+      <c r="C29" s="80">
         <f>0.1067424*100</f>
         <v>10.674239999999999</v>
       </c>
-      <c r="D29" s="83">
-        <v>0</v>
-      </c>
-      <c r="E29" s="83">
-        <v>0</v>
-      </c>
-      <c r="F29" s="83">
-        <v>0</v>
-      </c>
-      <c r="G29" s="83">
-        <v>0</v>
-      </c>
-      <c r="H29" s="83">
+      <c r="D29" s="80">
+        <v>0</v>
+      </c>
+      <c r="E29" s="80">
+        <v>0</v>
+      </c>
+      <c r="F29" s="80">
+        <v>0</v>
+      </c>
+      <c r="G29" s="80">
+        <v>0</v>
+      </c>
+      <c r="H29" s="80">
         <v>100</v>
       </c>
-      <c r="I29" s="83">
+      <c r="I29" s="80">
         <v>100</v>
       </c>
-      <c r="J29" s="83">
-        <v>0</v>
-      </c>
-      <c r="K29" s="91">
+      <c r="J29" s="80">
+        <v>0</v>
+      </c>
+      <c r="K29" s="88">
         <v>0</v>
       </c>
       <c r="L29" s="32"/>
@@ -6237,32 +6178,32 @@
       <c r="B30" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="83">
+      <c r="C30" s="80">
         <f>0.2369604*100</f>
         <v>23.69604</v>
       </c>
-      <c r="D30" s="83">
-        <v>0</v>
-      </c>
-      <c r="E30" s="83">
-        <v>0</v>
-      </c>
-      <c r="F30" s="83">
-        <v>0</v>
-      </c>
-      <c r="G30" s="83">
-        <v>0</v>
-      </c>
-      <c r="H30" s="83">
-        <v>0</v>
-      </c>
-      <c r="I30" s="83">
-        <v>0</v>
-      </c>
-      <c r="J30" s="83">
+      <c r="D30" s="80">
+        <v>0</v>
+      </c>
+      <c r="E30" s="80">
+        <v>0</v>
+      </c>
+      <c r="F30" s="80">
+        <v>0</v>
+      </c>
+      <c r="G30" s="80">
+        <v>0</v>
+      </c>
+      <c r="H30" s="80">
+        <v>0</v>
+      </c>
+      <c r="I30" s="80">
+        <v>0</v>
+      </c>
+      <c r="J30" s="80">
         <v>100</v>
       </c>
-      <c r="K30" s="91">
+      <c r="K30" s="88">
         <v>100</v>
       </c>
       <c r="L30" s="32"/>
@@ -6274,39 +6215,39 @@
       <c r="B31" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="C31" s="92">
+      <c r="C31" s="89">
         <f>SUM($C$27:$C$30)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="D31" s="92">
+      <c r="D31" s="89">
         <f>SUM($D$27:$D$30)</f>
         <v>100</v>
       </c>
-      <c r="E31" s="92">
+      <c r="E31" s="89">
         <f>SUM($E$27:$E$30)</f>
         <v>100</v>
       </c>
-      <c r="F31" s="92">
+      <c r="F31" s="89">
         <f>SUM($F$27:$F$30)</f>
         <v>100</v>
       </c>
-      <c r="G31" s="92">
+      <c r="G31" s="89">
         <f>SUM($G$27:$G$30)</f>
         <v>100</v>
       </c>
-      <c r="H31" s="92">
+      <c r="H31" s="89">
         <f>SUM($H$27:$H$30)</f>
         <v>100</v>
       </c>
-      <c r="I31" s="92">
+      <c r="I31" s="89">
         <f>SUM($I$27:$I$30)</f>
         <v>100</v>
       </c>
-      <c r="J31" s="92">
+      <c r="J31" s="89">
         <f>SUM($J$27:$J$30)</f>
         <v>100</v>
       </c>
-      <c r="K31" s="86">
+      <c r="K31" s="83">
         <f>SUM($K$27:$K$30)</f>
         <v>100</v>
       </c>
@@ -6316,16 +6257,16 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="32"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="89"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
       <c r="L32" s="32"/>
       <c r="M32" s="32"/>
       <c r="N32" s="32"/>
@@ -6348,7 +6289,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="32"/>
-      <c r="B34" s="87" t="s">
+      <c r="B34" s="84" t="s">
         <v>152</v>
       </c>
       <c r="C34" s="51"/>
@@ -6366,7 +6307,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="32"/>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="85" t="s">
         <v>153</v>
       </c>
       <c r="C35" s="51"/>
@@ -6445,51 +6386,51 @@
       <c r="B38" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="83">
+      <c r="C38" s="80">
         <f t="shared" ref="C38:N38" si="0">0.08091196*100</f>
         <v>8.0911960000000001</v>
       </c>
-      <c r="D38" s="83">
+      <c r="D38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="E38" s="83">
+      <c r="E38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="F38" s="83">
+      <c r="F38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="G38" s="83">
+      <c r="G38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="H38" s="83">
+      <c r="H38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="I38" s="83">
+      <c r="I38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="J38" s="83">
+      <c r="J38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="K38" s="83">
+      <c r="K38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="L38" s="83">
+      <c r="L38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="M38" s="83">
+      <c r="M38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
-      <c r="N38" s="83">
+      <c r="N38" s="80">
         <f t="shared" si="0"/>
         <v>8.0911960000000001</v>
       </c>
@@ -6499,51 +6440,51 @@
       <c r="B39" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="83">
+      <c r="C39" s="80">
         <f t="shared" ref="C39:N39" si="1">100*0.1549026</f>
         <v>15.490259999999999</v>
       </c>
-      <c r="D39" s="83">
+      <c r="D39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="E39" s="83">
+      <c r="E39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="F39" s="83">
+      <c r="F39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="G39" s="83">
+      <c r="G39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="H39" s="83">
+      <c r="H39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="I39" s="83">
+      <c r="I39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="J39" s="83">
+      <c r="J39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="K39" s="83">
+      <c r="K39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="L39" s="83">
+      <c r="L39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="M39" s="83">
+      <c r="M39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
-      <c r="N39" s="83">
+      <c r="N39" s="80">
         <f t="shared" si="1"/>
         <v>15.490259999999999</v>
       </c>
@@ -6553,51 +6494,51 @@
       <c r="B40" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="80">
         <f t="shared" ref="C40:N40" si="2">100*0.214183</f>
         <v>21.418300000000002</v>
       </c>
-      <c r="D40" s="83">
+      <c r="D40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="E40" s="83">
+      <c r="E40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="F40" s="83">
+      <c r="F40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="G40" s="83">
+      <c r="G40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="H40" s="83">
+      <c r="H40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="I40" s="83">
+      <c r="I40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="J40" s="83">
+      <c r="J40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="K40" s="83">
+      <c r="K40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="L40" s="83">
+      <c r="L40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="M40" s="83">
+      <c r="M40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
-      <c r="N40" s="83">
+      <c r="N40" s="80">
         <f t="shared" si="2"/>
         <v>21.418300000000002</v>
       </c>
@@ -6607,51 +6548,51 @@
       <c r="B41" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="85">
+      <c r="C41" s="82">
         <f t="shared" ref="C41:N41" si="3">100*0.1046608</f>
         <v>10.46608</v>
       </c>
-      <c r="D41" s="85">
+      <c r="D41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="E41" s="85">
+      <c r="E41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="F41" s="85">
+      <c r="F41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="G41" s="85">
+      <c r="G41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="H41" s="85">
+      <c r="H41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="I41" s="85">
+      <c r="I41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="J41" s="85">
+      <c r="J41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="K41" s="85">
+      <c r="K41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="L41" s="85">
+      <c r="L41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="M41" s="85">
+      <c r="M41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
-      <c r="N41" s="85">
+      <c r="N41" s="82">
         <f t="shared" si="3"/>
         <v>10.46608</v>
       </c>
@@ -6687,7 +6628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D20" sqref="D20:O21"/>
     </sheetView>
   </sheetViews>
@@ -6751,7 +6692,7 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
-      <c r="C4" s="93"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
@@ -6767,10 +6708,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="92" t="s">
         <v>158</v>
       </c>
       <c r="D5" s="38" t="s">
@@ -7114,7 +7055,7 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
-      <c r="C13" s="93"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
@@ -7130,10 +7071,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="92" t="s">
         <v>158</v>
       </c>
       <c r="D14" s="38" t="s">
@@ -7477,7 +7418,7 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
-      <c r="C22" s="93"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
       <c r="F22" s="36"/>
@@ -7493,10 +7434,10 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="32"/>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="92" t="s">
         <v>158</v>
       </c>
       <c r="D23" s="38" t="s">
@@ -7840,7 +7781,7 @@
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="32"/>
       <c r="B31" s="32"/>
-      <c r="C31" s="93"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="36"/>
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
@@ -7856,10 +7797,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="32"/>
-      <c r="B32" s="94" t="s">
+      <c r="B32" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="95" t="s">
+      <c r="C32" s="92" t="s">
         <v>158</v>
       </c>
       <c r="D32" s="38" t="s">

</xml_diff>